<commit_message>
Snowflake Pushdown Working Demo
</commit_message>
<xml_diff>
--- a/test/testcases/testcase24_snowflake_snowflake_etljob.xlsx
+++ b/test/testcases/testcase24_snowflake_snowflake_etljob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA8F9BC-F658-4B9D-B99A-560915FB9E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F162E551-BA09-4063-B7C0-35817A259AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -164,13 +164,16 @@
     <t>patienttgt</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>source_to_target</t>
   </si>
   <si>
     <t>SAMPLE_TGT_PATIENTS</t>
+  </si>
+  <si>
+    <t>BIRTHDATE,DEATHDATE</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +668,9 @@
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -729,7 +734,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,7 +759,9 @@
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -785,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -793,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>